<commit_message>
CO2 aralikli MTV modeli eklendi
</commit_message>
<xml_diff>
--- a/r_input/mtv_oranlari.xlsx
+++ b/r_input/mtv_oranlari.xlsx
@@ -1,25 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2253CDC7-FADD-45D1-A5A0-4E13C10E0878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE67252F-1787-4D77-B2F4-6575AD9F434D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="degiskenler" sheetId="4" r:id="rId1"/>
     <sheet name="OTV_grubuna_dayali_MTV" sheetId="1" r:id="rId2"/>
-    <sheet name="2020_mtv" sheetId="3" r:id="rId3"/>
-    <sheet name="eski_model" sheetId="2" r:id="rId4"/>
+    <sheet name="co2_araliklari" sheetId="5" r:id="rId3"/>
+    <sheet name="2020_mtv" sheetId="3" r:id="rId4"/>
+    <sheet name="otv_grubu_co2_araliklari" sheetId="6" r:id="rId5"/>
+    <sheet name="eski_modeli (arsiv)" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>1-3 age</t>
   </si>
@@ -196,16 +209,51 @@
   </si>
   <si>
     <t>co2_tax</t>
+  </si>
+  <si>
+    <t>co2_min</t>
+  </si>
+  <si>
+    <t>co2_max</t>
+  </si>
+  <si>
+    <t>co2_grubu</t>
+  </si>
+  <si>
+    <t>satis_fiyati_min</t>
+  </si>
+  <si>
+    <t>vergi_matrahi</t>
+  </si>
+  <si>
+    <t>co2_grubu_1</t>
+  </si>
+  <si>
+    <t>co2_grubu_2</t>
+  </si>
+  <si>
+    <t>co2_grubu_3</t>
+  </si>
+  <si>
+    <t>co2_grubu_4</t>
+  </si>
+  <si>
+    <t>co2_grubu_5</t>
+  </si>
+  <si>
+    <t>mevcut_otv_grubu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,6 +317,13 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -308,7 +363,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -328,8 +383,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -347,8 +403,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="İzlenen Köprü" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="İzlenen Köprü" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="İzlenen Köprü" xfId="6" builtinId="9" hidden="1"/>
@@ -368,6 +425,7 @@
     <cellStyle name="Köprü" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Köprü" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Virgül" xfId="19" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -380,6 +438,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="yeni_degiskenler"/>
+      <sheetName val="mevcut_degiskenler"/>
+      <sheetName val="yeni_otv"/>
+      <sheetName val="ice_mevcut"/>
+      <sheetName val="ice_eski"/>
+      <sheetName val="hybrid"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="B3">
+            <v>85000</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>130000</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>170000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -709,7 +806,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -828,6 +925,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EBF5AF-2DC9-47C4-B504-74C43DBA0314}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>96</v>
+      </c>
+      <c r="B3">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>126</v>
+      </c>
+      <c r="B5">
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>141</v>
+      </c>
+      <c r="B6">
+        <v>9999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41E080A-FFE8-4F1B-B1F2-126B6A5970E8}">
   <dimension ref="A1:AI21"/>
   <sheetViews>
@@ -3101,12 +3283,262 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8A912B-ADD4-4D63-9B17-9F969586F6B8}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="6" max="10" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1600</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>[1]mevcut_degiskenler!B3</f>
+        <v>85000</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1200</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1400</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1600</v>
+      </c>
+      <c r="I2" s="11">
+        <v>2000</v>
+      </c>
+      <c r="J2" s="11">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1600</v>
+      </c>
+      <c r="D3">
+        <v>145435</v>
+      </c>
+      <c r="E3">
+        <f>[1]mevcut_degiskenler!B4</f>
+        <v>130000</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1800</v>
+      </c>
+      <c r="G3" s="11">
+        <v>2000</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2200</v>
+      </c>
+      <c r="I3" s="11">
+        <v>2400</v>
+      </c>
+      <c r="J3" s="11">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1600</v>
+      </c>
+      <c r="D4">
+        <v>230100</v>
+      </c>
+      <c r="E4">
+        <v>99999999</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2400</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2600</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2800</v>
+      </c>
+      <c r="I4" s="11">
+        <v>3000</v>
+      </c>
+      <c r="J4" s="11">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1601</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>[1]mevcut_degiskenler!B5</f>
+        <v>170000</v>
+      </c>
+      <c r="F5" s="11">
+        <v>4000</v>
+      </c>
+      <c r="G5" s="11">
+        <v>4600</v>
+      </c>
+      <c r="H5" s="11">
+        <v>5200</v>
+      </c>
+      <c r="I5" s="11">
+        <v>5800</v>
+      </c>
+      <c r="J5" s="11">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1601</v>
+      </c>
+      <c r="C6">
+        <v>2000</v>
+      </c>
+      <c r="D6">
+        <v>461379.99999999988</v>
+      </c>
+      <c r="E6">
+        <v>99999999</v>
+      </c>
+      <c r="F6" s="11">
+        <v>6000</v>
+      </c>
+      <c r="G6" s="11">
+        <v>6600</v>
+      </c>
+      <c r="H6" s="11">
+        <v>7200</v>
+      </c>
+      <c r="I6" s="11">
+        <v>7800</v>
+      </c>
+      <c r="J6" s="11">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2001</v>
+      </c>
+      <c r="C7">
+        <v>999999</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>99999999</v>
+      </c>
+      <c r="F7" s="11">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="11">
+        <v>14000</v>
+      </c>
+      <c r="H7" s="11">
+        <v>18000</v>
+      </c>
+      <c r="I7" s="11">
+        <v>22000</v>
+      </c>
+      <c r="J7" s="11">
+        <v>26000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>